<commit_message>
revise the data cleaning file
</commit_message>
<xml_diff>
--- a/Huimin/Variable_Analysis_11.07.xlsx
+++ b/Huimin/Variable_Analysis_11.07.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop2\Documents\Bootcamp\Kaggle-House-Prices\Huimin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D386B873-3388-4AA8-8FAE-2667BE945630}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D026AD2-119D-4852-AB19-E5C7845FEFEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{62575EAA-3102-4243-B684-290054381A1F}"/>
+    <workbookView xWindow="-105" yWindow="1155" windowWidth="15570" windowHeight="11385" xr2:uid="{62575EAA-3102-4243-B684-290054381A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="136">
   <si>
     <t>categorical</t>
   </si>
@@ -435,10 +435,13 @@
     <t>categorical/ordinal?</t>
   </si>
   <si>
-    <t>numerical/</t>
-  </si>
-  <si>
     <t>ordinal/categorical</t>
+  </si>
+  <si>
+    <t>MissingValue</t>
+  </si>
+  <si>
+    <t>drop function</t>
   </si>
 </sst>
 </file>
@@ -961,10 +964,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6D78E1-BCBA-40BA-A99D-C281CEF30B87}">
-  <dimension ref="A1:I82"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="129" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +980,7 @@
     <col min="7" max="16384" width="16.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>98</v>
       </c>
@@ -1002,8 +1006,12 @@
         <v>93</v>
       </c>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="J1" s="1"/>
+      <c r="K1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1021,8 +1029,12 @@
       <c r="I2" s="24" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J2"/>
+      <c r="K2" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1062,7 +1074,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1130,7 +1142,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1154,7 +1166,7 @@
       </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1174,7 +1186,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1196,7 +1208,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1214,7 +1226,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1232,7 +1244,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1250,7 +1262,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1268,7 +1280,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1286,7 +1298,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1304,7 +1316,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1322,7 +1334,7 @@
       <c r="G17" s="13"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1342,7 +1354,7 @@
       </c>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1386,7 +1398,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -1406,7 +1418,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1426,7 +1438,7 @@
       </c>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -1448,7 +1460,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -1470,7 +1482,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -1492,7 +1504,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -1560,7 +1572,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>28</v>
       </c>
@@ -1582,7 +1594,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -1602,7 +1614,7 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>30</v>
       </c>
@@ -1620,7 +1632,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -1640,7 +1652,7 @@
       <c r="G32" s="12"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>32</v>
       </c>
@@ -1688,7 +1700,7 @@
       </c>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>34</v>
       </c>
@@ -1712,7 +1724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -1732,7 +1744,7 @@
       </c>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>36</v>
       </c>
@@ -1756,7 +1768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -1776,7 +1788,7 @@
       </c>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>38</v>
       </c>
@@ -1787,14 +1799,14 @@
         <v>1</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
       <c r="G39" s="27"/>
       <c r="H39" s="11"/>
     </row>
-    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -1814,7 +1826,7 @@
       </c>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>40</v>
       </c>
@@ -1832,7 +1844,7 @@
       <c r="G41" s="13"/>
       <c r="H41" s="11"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -1850,7 +1862,7 @@
       <c r="G42" s="13"/>
       <c r="H42" s="11"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>42</v>
       </c>
@@ -1870,7 +1882,7 @@
       </c>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -1892,7 +1904,7 @@
       </c>
       <c r="H44" s="11"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>44</v>
       </c>
@@ -1910,7 +1922,7 @@
       <c r="G45" s="13"/>
       <c r="H45" s="11"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -1928,7 +1940,7 @@
       <c r="G46" s="13"/>
       <c r="H46" s="11"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>46</v>
       </c>
@@ -1946,7 +1958,7 @@
       <c r="G47" s="13"/>
       <c r="H47" s="11"/>
     </row>
-    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -1966,7 +1978,7 @@
       </c>
       <c r="H48" s="11"/>
     </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>48</v>
       </c>
@@ -1986,7 +1998,7 @@
       </c>
       <c r="H49" s="11"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2006,7 +2018,7 @@
       </c>
       <c r="H50" s="11"/>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>50</v>
       </c>
@@ -2026,7 +2038,7 @@
       </c>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -2046,7 +2058,7 @@
       </c>
       <c r="H52" s="11"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>52</v>
       </c>
@@ -2064,7 +2076,7 @@
       <c r="G53" s="13"/>
       <c r="H53" s="11"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -2082,7 +2094,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="11"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>54</v>
       </c>
@@ -2100,7 +2112,7 @@
       <c r="G55" s="13"/>
       <c r="H55" s="11"/>
     </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -2120,7 +2132,7 @@
       </c>
       <c r="H56" s="11"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>56</v>
       </c>
@@ -2138,7 +2150,7 @@
       <c r="G57" s="13"/>
       <c r="H57" s="11"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -2156,7 +2168,7 @@
       <c r="G58" s="13"/>
       <c r="H58" s="11"/>
     </row>
-    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>58</v>
       </c>
@@ -2178,7 +2190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -2202,7 +2214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>60</v>
       </c>
@@ -2224,7 +2236,7 @@
       <c r="G61" s="13"/>
       <c r="H61" s="11"/>
     </row>
-    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -2246,7 +2258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>62</v>
       </c>
@@ -2266,7 +2278,7 @@
       </c>
       <c r="H63" s="11"/>
     </row>
-    <row r="64" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -2286,7 +2298,7 @@
       </c>
       <c r="H64" s="11"/>
     </row>
-    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>64</v>
       </c>
@@ -2310,7 +2322,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -2334,7 +2346,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>66</v>
       </c>
@@ -2352,7 +2364,7 @@
       <c r="G67" s="13"/>
       <c r="H67" s="11"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -2370,7 +2382,7 @@
       <c r="G68" s="13"/>
       <c r="H68" s="11"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>68</v>
       </c>
@@ -2388,7 +2400,7 @@
       <c r="G69" s="13"/>
       <c r="H69" s="11"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -2406,7 +2418,7 @@
       <c r="G70" s="13"/>
       <c r="H70" s="11"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>70</v>
       </c>
@@ -2424,7 +2436,7 @@
       <c r="G71" s="13"/>
       <c r="H71" s="11"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -2442,7 +2454,7 @@
       <c r="G72" s="13"/>
       <c r="H72" s="11"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>72</v>
       </c>
@@ -2460,7 +2472,7 @@
       <c r="G73" s="13"/>
       <c r="H73" s="11"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -2480,7 +2492,7 @@
       <c r="G74" s="13"/>
       <c r="H74" s="11"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>74</v>
       </c>
@@ -2500,7 +2512,7 @@
       <c r="G75" s="13"/>
       <c r="H75" s="11"/>
     </row>
-    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -2522,7 +2534,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>76</v>
       </c>
@@ -2588,10 +2600,10 @@
         <v>85</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="14"/>
@@ -2620,7 +2632,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -2628,10 +2640,10 @@
         <v>87</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="14"/>
@@ -2639,7 +2651,18 @@
       <c r="H82" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F82" xr:uid="{AE415309-5D1E-4E06-A995-E399D58F3622}"/>
+  <autoFilter ref="A1:K82" xr:uid="{CF4CDAFE-58F0-4BEC-B603-2FBAADF9F560}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="categorical/ordinal?"/>
+        <filter val="categorical/Ordinal? Not sure. If exposure more, then price more. Then ordinal. Otherwise, categorical"/>
+        <filter val="date"/>
+        <filter val="if there is missing? It means it does not know the type. We can  look at the neighborhood then determine if what type it is."/>
+        <filter val="ordinal/categorical"/>
+        <filter val="use the average of the type average or median"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>